<commit_message>
ui and price fix
</commit_message>
<xml_diff>
--- a/m2matik/public/data/priser-til-beregning.xlsx
+++ b/m2matik/public/data/priser-til-beregning.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dropbox\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dropbox\_M W A\Prisberegner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71419898-87A4-4BEB-B921-10B06890E7C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E0268104-1A59-43DC-ACE7-AD615E4A88AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9720" yWindow="2400" windowWidth="27390" windowHeight="17050" xr2:uid="{0CE7EE46-CFF7-4A62-9690-1D9D1196770E}"/>
+    <workbookView xWindow="8130" yWindow="2490" windowWidth="27390" windowHeight="17050" xr2:uid="{0CE7EE46-CFF7-4A62-9690-1D9D1196770E}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>Renovering</t>
   </si>
@@ -129,6 +129,24 @@
   </si>
   <si>
     <t>prisinddex hældning</t>
+  </si>
+  <si>
+    <t>Terasse</t>
+  </si>
+  <si>
+    <t>faktor ved hævet</t>
+  </si>
+  <si>
+    <t>faktor  ved værn</t>
+  </si>
+  <si>
+    <t>tilvalg trappe</t>
+  </si>
+  <si>
+    <t>Gulve</t>
+  </si>
+  <si>
+    <t>tillæg gulvvarme</t>
   </si>
 </sst>
 </file>
@@ -514,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D51C9524-2949-4525-A197-7F7CFC389C3D}">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -921,19 +939,19 @@
         <v>2</v>
       </c>
       <c r="F26" s="2">
-        <f t="shared" ref="F26:F28" si="12">($C26*80*D26)+$B26</f>
+        <f t="shared" ref="F26" si="12">($C26*80*D26)+$B26</f>
         <v>170000</v>
       </c>
       <c r="G26" s="2">
-        <f t="shared" ref="G26:G28" si="13">($C26*80*E26)+$B26</f>
+        <f t="shared" ref="G26" si="13">($C26*80*E26)+$B26</f>
         <v>430000</v>
       </c>
       <c r="H26" s="2">
-        <f t="shared" ref="H26:H28" si="14">($C26*200*D26)+$B26</f>
+        <f t="shared" ref="H26" si="14">($C26*200*D26)+$B26</f>
         <v>380000</v>
       </c>
       <c r="I26" s="2">
-        <f t="shared" ref="I26:I28" si="15">($C26*200*E26)+$B26</f>
+        <f t="shared" ref="I26" si="15">($C26*200*E26)+$B26</f>
         <v>1030000</v>
       </c>
     </row>
@@ -988,6 +1006,126 @@
         <v>2000</v>
       </c>
     </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>10000</v>
+      </c>
+      <c r="C33">
+        <v>3000</v>
+      </c>
+      <c r="D33">
+        <v>0.6</v>
+      </c>
+      <c r="E33">
+        <v>1.4</v>
+      </c>
+      <c r="F33" s="2">
+        <f>($C33*20*D33)+$B33</f>
+        <v>46000</v>
+      </c>
+      <c r="G33" s="2">
+        <f>($C33*20*E33)+$B33</f>
+        <v>94000</v>
+      </c>
+      <c r="H33" s="2">
+        <f>($C33*60*D33)+$B33</f>
+        <v>118000</v>
+      </c>
+      <c r="I33" s="2">
+        <f>($C33*60*E33)+$B33</f>
+        <v>261999.99999999997</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>35</v>
+      </c>
+      <c r="B39">
+        <v>10000</v>
+      </c>
+      <c r="C39">
+        <v>1000</v>
+      </c>
+      <c r="D39">
+        <v>0.4</v>
+      </c>
+      <c r="E39">
+        <v>2</v>
+      </c>
+      <c r="F39" s="2">
+        <f t="shared" ref="F39" si="16">($C39*80*D39)+$B39</f>
+        <v>42000</v>
+      </c>
+      <c r="G39" s="2">
+        <f t="shared" ref="G39" si="17">($C39*80*E39)+$B39</f>
+        <v>170000</v>
+      </c>
+      <c r="H39" s="2">
+        <f t="shared" ref="H39" si="18">($C39*200*D39)+$B39</f>
+        <v>90000</v>
+      </c>
+      <c r="I39" s="2">
+        <f t="shared" ref="I39" si="19">($C39*200*E39)+$B39</f>
+        <v>410000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>36</v>
+      </c>
+      <c r="C40">
+        <v>500</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40" s="2">
+        <f t="shared" ref="F40" si="20">($C40*80*D40)+$B40</f>
+        <v>40000</v>
+      </c>
+      <c r="G40" s="2">
+        <f t="shared" ref="G40" si="21">($C40*80*E40)+$B40</f>
+        <v>40000</v>
+      </c>
+      <c r="H40" s="2">
+        <f t="shared" ref="H40" si="22">($C40*200*D40)+$B40</f>
+        <v>100000</v>
+      </c>
+      <c r="I40" s="2">
+        <f t="shared" ref="I40" si="23">($C40*200*E40)+$B40</f>
+        <v>100000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>